<commit_message>
adjusted to run on multiple platforms
</commit_message>
<xml_diff>
--- a/generated_sheets/multiprocessing/testing purposes - para2.xlsx
+++ b/generated_sheets/multiprocessing/testing purposes - para2.xlsx
@@ -2482,44 +2482,44 @@
       </c>
       <c r="D4" s="45" t="inlineStr">
         <is>
-          <t>1380,4065</t>
+          <t>3653,4721</t>
         </is>
       </c>
       <c r="E4" s="46" t="n">
-        <v>0.1248788833618164</v>
+        <v>1.1406090259552</v>
       </c>
       <c r="F4" s="47" t="n">
-        <v>0.100003719329834</v>
+        <v>0.09375214576721191</v>
       </c>
       <c r="G4" s="47" t="n">
-        <v>0.02467012405395508</v>
+        <v>0.03125119209289551</v>
       </c>
       <c r="H4" s="48" t="n">
-        <v>988</v>
+        <v>1056.6</v>
       </c>
       <c r="I4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="J4" s="44" t="n">
-        <v>1000.5</v>
+        <v>1003.5</v>
       </c>
       <c r="K4" s="49" t="n">
-        <v>2516.1</v>
+        <v>2514.1</v>
       </c>
       <c r="L4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="44" t="n">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="N4" s="49" t="n">
-        <v>2547.9</v>
+        <v>2526.1</v>
       </c>
       <c r="O4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="P4" s="44" t="n">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="Q4" s="45">
         <f>SUM(H4:P4)</f>
@@ -2530,31 +2530,31 @@
         <v/>
       </c>
       <c r="S4" s="45" t="n">
-        <v>949.5</v>
+        <v>1021.5</v>
       </c>
       <c r="T4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="U4" s="44" t="n">
-        <v>1000.5</v>
+        <v>1003.5</v>
       </c>
       <c r="V4" s="49" t="n">
-        <v>2535.7</v>
+        <v>2531.8</v>
       </c>
       <c r="W4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="X4" s="44" t="n">
-        <v>646</v>
+        <v>653</v>
       </c>
       <c r="Y4" s="49" t="n">
-        <v>2566.8</v>
+        <v>2543.5</v>
       </c>
       <c r="Z4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="AA4" s="44" t="n">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="AB4" s="45">
         <f>SUM(S4:AA4)</f>
@@ -2569,31 +2569,31 @@
         <v/>
       </c>
       <c r="AE4" s="45" t="n">
-        <v>876</v>
+        <v>939</v>
       </c>
       <c r="AF4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="AG4" s="44" t="n">
-        <v>1000.5</v>
+        <v>1003.5</v>
       </c>
       <c r="AH4" s="49" t="n">
-        <v>2582.2</v>
+        <v>2581.3</v>
       </c>
       <c r="AI4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="AJ4" s="44" t="n">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="AK4" s="49" t="n">
-        <v>2593.8</v>
+        <v>2576.5</v>
       </c>
       <c r="AL4" s="44" t="n">
         <v>0</v>
       </c>
       <c r="AM4" s="44" t="n">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="AN4" s="45">
         <f>SUM(AE4:AM4)</f>
@@ -2658,44 +2658,44 @@
       </c>
       <c r="D5" s="55" t="inlineStr">
         <is>
-          <t>7472,3577</t>
+          <t>4920,6269</t>
         </is>
       </c>
       <c r="E5" s="56" t="n">
-        <v>0.1001849174499512</v>
+        <v>0.1406242847442627</v>
       </c>
       <c r="F5" s="57" t="n">
-        <v>0.107086181640625</v>
+        <v>0.0937502384185791</v>
       </c>
       <c r="G5" s="57" t="n">
-        <v>0.0325160026550293</v>
+        <v>0.03124880790710449</v>
       </c>
       <c r="H5" s="58" t="n">
-        <v>1001.9</v>
+        <v>1039.9</v>
       </c>
       <c r="I5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="59" t="n">
-        <v>988.5</v>
+        <v>996</v>
       </c>
       <c r="K5" s="60" t="n">
-        <v>2573.2</v>
+        <v>2558.1</v>
       </c>
       <c r="L5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="59" t="n">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="N5" s="60" t="n">
-        <v>2599</v>
+        <v>2536.6</v>
       </c>
       <c r="O5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="P5" s="59" t="n">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="Q5" s="61">
         <f>SUM(H5:P5)</f>
@@ -2706,31 +2706,31 @@
         <v/>
       </c>
       <c r="S5" s="61" t="n">
-        <v>973.5</v>
+        <v>1000.5</v>
       </c>
       <c r="T5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="U5" s="59" t="n">
-        <v>988.5</v>
+        <v>996</v>
       </c>
       <c r="V5" s="60" t="n">
-        <v>2585.1</v>
+        <v>2581.6</v>
       </c>
       <c r="W5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="X5" s="59" t="n">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="Y5" s="60" t="n">
-        <v>2615.5</v>
+        <v>2552.5</v>
       </c>
       <c r="Z5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="AA5" s="59" t="n">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="AB5" s="61">
         <f>SUM(S5:AA5)</f>
@@ -2745,31 +2745,31 @@
         <v/>
       </c>
       <c r="AE5" s="61" t="n">
-        <v>909</v>
+        <v>928.5</v>
       </c>
       <c r="AF5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="AG5" s="59" t="n">
-        <v>988.5</v>
+        <v>996</v>
       </c>
       <c r="AH5" s="60" t="n">
-        <v>2627.1</v>
+        <v>2599.6</v>
       </c>
       <c r="AI5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="AJ5" s="59" t="n">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="AK5" s="60" t="n">
-        <v>2638</v>
+        <v>2606.5</v>
       </c>
       <c r="AL5" s="59" t="n">
         <v>0</v>
       </c>
       <c r="AM5" s="59" t="n">
-        <v>653</v>
+        <v>667</v>
       </c>
       <c r="AN5" s="61">
         <f>SUM(AE5:AM5)</f>

</xml_diff>